<commit_message>
Added percentile score and format
</commit_message>
<xml_diff>
--- a/CAPM Model/capm_stocks.xlsx
+++ b/CAPM Model/capm_stocks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>Ticker</t>
   </si>
@@ -31,6 +31,9 @@
     <t>CAPM Expected Return</t>
   </si>
   <si>
+    <t>CAPM Percentile</t>
+  </si>
+  <si>
     <t>K</t>
   </si>
   <si>
@@ -49,136 +52,136 @@
     <t>LMT</t>
   </si>
   <si>
+    <t>ATVI</t>
+  </si>
+  <si>
     <t>SJM</t>
   </si>
   <si>
     <t>KHC</t>
   </si>
   <si>
-    <t>ATVI</t>
+    <t>GIS</t>
+  </si>
+  <si>
+    <t>BMY</t>
+  </si>
+  <si>
+    <t>DUK</t>
+  </si>
+  <si>
+    <t>MRK</t>
+  </si>
+  <si>
+    <t>VZ</t>
+  </si>
+  <si>
+    <t>CMS</t>
   </si>
   <si>
     <t>WEC</t>
   </si>
   <si>
-    <t>DUK</t>
-  </si>
-  <si>
-    <t>CMS</t>
-  </si>
-  <si>
     <t>CHD</t>
   </si>
   <si>
+    <t>JNJ</t>
+  </si>
+  <si>
     <t>ED</t>
   </si>
   <si>
-    <t>GIS</t>
-  </si>
-  <si>
     <t>CLX</t>
   </si>
   <si>
-    <t>BMY</t>
-  </si>
-  <si>
-    <t>VZ</t>
-  </si>
-  <si>
-    <t>MRK</t>
+    <t>NOC</t>
   </si>
   <si>
     <t>MO</t>
   </si>
   <si>
-    <t>JNJ</t>
+    <t>CTXS</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
   <si>
     <t>PNW</t>
   </si>
   <si>
-    <t>NOC</t>
-  </si>
-  <si>
-    <t>KR</t>
-  </si>
-  <si>
-    <t>SO</t>
-  </si>
-  <si>
-    <t>D</t>
+    <t>ABBV</t>
+  </si>
+  <si>
+    <t>DTE</t>
   </si>
   <si>
     <t>ES</t>
   </si>
   <si>
-    <t>DTE</t>
-  </si>
-  <si>
     <t>XEL</t>
   </si>
   <si>
+    <t>HSY</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
     <t>CL</t>
   </si>
   <si>
-    <t>ABBV</t>
-  </si>
-  <si>
-    <t>PM</t>
-  </si>
-  <si>
-    <t>HSY</t>
+    <t>CAG</t>
+  </si>
+  <si>
+    <t>AMGN</t>
   </si>
   <si>
     <t>LNT</t>
   </si>
   <si>
-    <t>CTXS</t>
-  </si>
-  <si>
-    <t>CAG</t>
+    <t>MKC</t>
   </si>
   <si>
     <t>AEE</t>
   </si>
   <si>
+    <t>AEP</t>
+  </si>
+  <si>
+    <t>LHX</t>
+  </si>
+  <si>
+    <t>PFE</t>
+  </si>
+  <si>
     <t>ETR</t>
   </si>
   <si>
-    <t>LHX</t>
-  </si>
-  <si>
-    <t>AMGN</t>
-  </si>
-  <si>
-    <t>PFE</t>
-  </si>
-  <si>
-    <t>AEP</t>
-  </si>
-  <si>
-    <t>MKC</t>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>BDX</t>
+  </si>
+  <si>
+    <t>ATO</t>
+  </si>
+  <si>
+    <t>WMT</t>
   </si>
   <si>
     <t>PEG</t>
   </si>
   <si>
-    <t>BDX</t>
+    <t>EVRG</t>
   </si>
   <si>
     <t>GILD</t>
-  </si>
-  <si>
-    <t>ATO</t>
-  </si>
-  <si>
-    <t>EVRG</t>
-  </si>
-  <si>
-    <t>FE</t>
-  </si>
-  <si>
-    <t>WMT</t>
   </si>
   <si>
     <t>NI</t>
@@ -548,7 +551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -559,9 +562,10 @@
     <col min="3" max="3" width="20.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,872 +581,1028 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2">
-        <v>72.61</v>
+        <v>71.08</v>
       </c>
       <c r="C2" s="3">
-        <v>2700</v>
+        <v>2758</v>
       </c>
       <c r="D2" s="3">
-        <v>0.06553536175633942</v>
+        <v>0.08870035571779128</v>
       </c>
       <c r="E2" s="3">
-        <v>3.048357508722241</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>3.153756251908614</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>42.2</v>
+        <v>43.71</v>
       </c>
       <c r="C3" s="3">
-        <v>4646</v>
+        <v>4485</v>
       </c>
       <c r="D3" s="3">
-        <v>0.097674601672391</v>
+        <v>0.1132492887889144</v>
       </c>
       <c r="E3" s="3">
-        <v>2.939661668616068</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>3.066231838469319</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.998003992015968</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>50.66</v>
+        <v>45.79</v>
       </c>
       <c r="C4" s="3">
-        <v>3870</v>
+        <v>4282</v>
       </c>
       <c r="D4" s="3">
-        <v>0.1579424046512712</v>
+        <v>0.1741485743328905</v>
       </c>
       <c r="E4" s="3">
-        <v>2.735834213665245</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>2.857365876046449</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.996007984031936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
-        <v>128.83</v>
+        <v>122.02</v>
       </c>
       <c r="C5" s="3">
-        <v>1521</v>
+        <v>1606</v>
       </c>
       <c r="D5" s="3">
-        <v>0.1936868202336957</v>
+        <v>0.2134716442446486</v>
       </c>
       <c r="E5" s="3">
-        <v>2.614945565054256</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>2.70890865666937</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.9940119760479043</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
-        <v>50.69</v>
+        <v>47.69</v>
       </c>
       <c r="C6" s="3">
-        <v>3868</v>
+        <v>4111</v>
       </c>
       <c r="D6" s="3">
-        <v>0.2199541805766312</v>
+        <v>0.2232343276931761</v>
       </c>
       <c r="E6" s="3">
-        <v>2.526108591706266</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>2.681869377386286</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.9920159680638723</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2">
-        <v>422.31</v>
+        <v>414.29</v>
       </c>
       <c r="C7" s="3">
-        <v>464</v>
+        <v>473</v>
       </c>
       <c r="D7" s="3">
-        <v>0.2197472755122611</v>
+        <v>0.2292362383235769</v>
       </c>
       <c r="E7" s="3">
-        <v>2.519005823380787</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>2.652703083666695</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.9900199600798403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
-        <v>140.81</v>
+        <v>76.02</v>
       </c>
       <c r="C8" s="3">
-        <v>1392</v>
+        <v>2579</v>
       </c>
       <c r="D8" s="3">
-        <v>0.2310166132725658</v>
+        <v>0.2396909437376558</v>
       </c>
       <c r="E8" s="3">
-        <v>2.488695123975125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>2.623031969423886</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.9880239520958084</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
-        <v>37.41</v>
+        <v>138.88</v>
       </c>
       <c r="C9" s="3">
-        <v>5241</v>
+        <v>1411</v>
       </c>
       <c r="D9" s="3">
-        <v>0.2368379336611547</v>
+        <v>0.245022749408747</v>
       </c>
       <c r="E9" s="3">
-        <v>2.46900724984314</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>2.603969142376192</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.9860279441117764</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2">
-        <v>78.62</v>
+        <v>34.71</v>
       </c>
       <c r="C10" s="3">
-        <v>2494</v>
+        <v>5649</v>
       </c>
       <c r="D10" s="3">
-        <v>0.2395575533233395</v>
+        <v>0.264706853981594</v>
       </c>
       <c r="E10" s="3">
-        <v>2.459809417389026</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>2.526239549760592</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.9840319361277444</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2">
-        <v>103.47</v>
+        <v>75.25</v>
       </c>
       <c r="C11" s="3">
-        <v>1895</v>
+        <v>2605</v>
       </c>
       <c r="D11" s="3">
-        <v>0.2427385905146336</v>
+        <v>0.2674146414974098</v>
       </c>
       <c r="E11" s="3">
-        <v>2.441478443394565</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>2.523911317224913</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.9820359281437127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2">
-        <v>107.68</v>
+        <v>71.52</v>
       </c>
       <c r="C12" s="3">
-        <v>1820</v>
+        <v>2741</v>
       </c>
       <c r="D12" s="3">
-        <v>0.2454713658271024</v>
+        <v>0.2696381502366168</v>
       </c>
       <c r="E12" s="3">
-        <v>2.439808732245073</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>2.51596159715834</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.9800399201596807</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2">
-        <v>68.11</v>
+        <v>106.11</v>
       </c>
       <c r="C13" s="3">
-        <v>2878</v>
+        <v>1847</v>
       </c>
       <c r="D13" s="3">
-        <v>0.2458730328885286</v>
+        <v>0.2726787676307889</v>
       </c>
       <c r="E13" s="3">
-        <v>2.43845028261158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>2.505090465110602</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.9780439121756487</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2">
-        <v>84.72</v>
+        <v>87.72</v>
       </c>
       <c r="C14" s="3">
-        <v>2314</v>
+        <v>2235</v>
       </c>
       <c r="D14" s="3">
-        <v>0.2460002900714585</v>
+        <v>0.276215451123147</v>
       </c>
       <c r="E14" s="3">
-        <v>2.438019895133711</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>2.485207900384821</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.9760479041916167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2">
-        <v>98.3</v>
+        <v>41.25</v>
       </c>
       <c r="C15" s="3">
-        <v>1994</v>
+        <v>4753</v>
       </c>
       <c r="D15" s="3">
-        <v>0.2528692842485769</v>
+        <v>0.2799406242435205</v>
       </c>
       <c r="E15" s="3">
-        <v>2.414788757909666</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>2.479127118883595</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.9740518962075848</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2">
-        <v>76.98</v>
+        <v>66.84</v>
       </c>
       <c r="C16" s="3">
-        <v>2547</v>
+        <v>2933</v>
       </c>
       <c r="D16" s="3">
-        <v>0.2541141142613633</v>
+        <v>0.2859287273733118</v>
       </c>
       <c r="E16" s="3">
-        <v>2.410578706757784</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>2.45771782879527</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.9720558882235529</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2">
-        <v>145.67</v>
+        <v>101.29</v>
       </c>
       <c r="C17" s="3">
-        <v>1346</v>
+        <v>1935</v>
       </c>
       <c r="D17" s="3">
-        <v>0.2608111225864119</v>
+        <v>0.2863431585303114</v>
       </c>
       <c r="E17" s="3">
-        <v>2.387929230665923</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>2.45623611135161</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.9700598802395209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2">
-        <v>67.2</v>
+        <v>76.54000000000001</v>
       </c>
       <c r="C18" s="3">
-        <v>2917</v>
+        <v>2561</v>
       </c>
       <c r="D18" s="3">
-        <v>0.2632206677263671</v>
+        <v>0.2889589811161166</v>
       </c>
       <c r="E18" s="3">
-        <v>2.379780079225339</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>2.446883749953478</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.9680638722554891</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2">
-        <v>42.53</v>
+        <v>167.6</v>
       </c>
       <c r="C19" s="3">
-        <v>4610</v>
+        <v>1169</v>
       </c>
       <c r="D19" s="3">
-        <v>0.2673130314958559</v>
+        <v>0.2875297132644146</v>
       </c>
       <c r="E19" s="3">
-        <v>2.365939586447459</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>2.44486911439588</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.9660678642714571</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2">
-        <v>86.88</v>
+        <v>97.41</v>
       </c>
       <c r="C20" s="3">
-        <v>2256</v>
+        <v>2012</v>
       </c>
       <c r="D20" s="3">
-        <v>0.2679955543475236</v>
+        <v>0.2896964359630358</v>
       </c>
       <c r="E20" s="3">
-        <v>2.35631122994163</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>2.444247124564348</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.9640718562874251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" s="2">
-        <v>45.12</v>
+        <v>141.77</v>
       </c>
       <c r="C21" s="3">
-        <v>4345</v>
+        <v>1383</v>
       </c>
       <c r="D21" s="3">
-        <v>0.2722274875529521</v>
+        <v>0.293152118551428</v>
       </c>
       <c r="E21" s="3">
-        <v>2.349318753746181</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>2.431892008197032</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.9620758483033931</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2">
-        <v>162.43</v>
+        <v>485.2</v>
       </c>
       <c r="C22" s="3">
-        <v>1207</v>
+        <v>404</v>
       </c>
       <c r="D22" s="3">
-        <v>0.2774251620244639</v>
+        <v>0.2953949540484385</v>
       </c>
       <c r="E22" s="3">
-        <v>2.331740068165716</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>2.416827138633183</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.9600798403193613</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B23" s="2">
-        <v>75.39</v>
+        <v>42.29</v>
       </c>
       <c r="C23" s="3">
-        <v>2600</v>
+        <v>4636</v>
       </c>
       <c r="D23" s="3">
-        <v>0.281045541850198</v>
+        <v>0.2986047845191899</v>
       </c>
       <c r="E23" s="3">
-        <v>2.319495838753649</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>2.412397068826704</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0.9580838323353293</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B24" s="2">
-        <v>480.93</v>
+        <v>103.53</v>
       </c>
       <c r="C24" s="3">
-        <v>407</v>
+        <v>1893</v>
       </c>
       <c r="D24" s="3">
-        <v>0.2841078886050449</v>
+        <v>0.3059641636003093</v>
       </c>
       <c r="E24" s="3">
-        <v>2.309138893347225</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>2.386085050111834</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.9560878243512974</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25" s="2">
-        <v>47.51</v>
+        <v>47.28</v>
       </c>
       <c r="C25" s="3">
-        <v>4127</v>
+        <v>4147</v>
       </c>
       <c r="D25" s="3">
-        <v>0.2858783136705478</v>
+        <v>0.304369296479734</v>
       </c>
       <c r="E25" s="3">
-        <v>2.303151264506515</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>2.384830878142886</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.9540918163672655</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2">
-        <v>77.58</v>
+        <v>77.25</v>
       </c>
       <c r="C26" s="3">
-        <v>2527</v>
+        <v>2538</v>
       </c>
       <c r="D26" s="3">
-        <v>0.2864021299172418</v>
+        <v>0.3092262956333047</v>
       </c>
       <c r="E26" s="3">
-        <v>2.301379702791166</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>2.374421935852269</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.9520958083832335</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B27" s="2">
-        <v>82.34</v>
+        <v>80.81999999999999</v>
       </c>
       <c r="C27" s="3">
-        <v>2381</v>
+        <v>2426</v>
       </c>
       <c r="D27" s="3">
-        <v>0.2919103836086254</v>
+        <v>0.3169031624095707</v>
       </c>
       <c r="E27" s="3">
-        <v>2.28275062929513</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>2.346974802057125</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.9500998003992016</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B28" s="2">
-        <v>90.77</v>
+        <v>73.63</v>
       </c>
       <c r="C28" s="3">
-        <v>2160</v>
+        <v>2663</v>
       </c>
       <c r="D28" s="3">
-        <v>0.2980891350148851</v>
+        <v>0.3179440699981383</v>
       </c>
       <c r="E28" s="3">
-        <v>2.261853913110651</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>2.343253240815483</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.9481037924151697</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B29" s="2">
-        <v>131.45</v>
+        <v>144.06</v>
       </c>
       <c r="C29" s="3">
-        <v>1491</v>
+        <v>1361</v>
       </c>
       <c r="D29" s="3">
-        <v>0.3034235454825603</v>
+        <v>0.320315512401274</v>
       </c>
       <c r="E29" s="3">
-        <v>2.243812782431468</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>2.334774612903432</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.9461077844311377</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B30" s="2">
-        <v>74.69</v>
+        <v>129.9</v>
       </c>
       <c r="C30" s="3">
-        <v>2625</v>
+        <v>1509</v>
       </c>
       <c r="D30" s="3">
-        <v>0.3036483860179547</v>
+        <v>0.3255546785049199</v>
       </c>
       <c r="E30" s="3">
-        <v>2.236088849089858</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>2.316043000487501</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0.9441117764471058</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B31" s="2">
-        <v>79</v>
+        <v>88.8</v>
       </c>
       <c r="C31" s="3">
-        <v>2482</v>
+        <v>2208</v>
       </c>
       <c r="D31" s="3">
-        <v>0.315543058727507</v>
+        <v>0.3283358418657169</v>
       </c>
       <c r="E31" s="3">
-        <v>2.202824237671907</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>2.306099495527125</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.9421157684630738</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B32" s="2">
-        <v>135.55</v>
+        <v>73.90000000000001</v>
       </c>
       <c r="C32" s="3">
-        <v>1446</v>
+        <v>2653</v>
       </c>
       <c r="D32" s="3">
-        <v>0.3164506341568617</v>
+        <v>0.3305068812930365</v>
       </c>
       <c r="E32" s="3">
-        <v>2.199754791287639</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>2.298337369210122</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0.940119760479042</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B33" s="2">
-        <v>95.48999999999999</v>
+        <v>219.89</v>
       </c>
       <c r="C33" s="3">
-        <v>2053</v>
+        <v>891</v>
       </c>
       <c r="D33" s="3">
-        <v>0.316574981790515</v>
+        <v>0.3321546213518931</v>
       </c>
       <c r="E33" s="3">
-        <v>2.199334243989679</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>2.292446197307169</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0.93812375249501</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B34" s="2">
-        <v>226.21</v>
+        <v>95.56</v>
       </c>
       <c r="C34" s="3">
-        <v>866</v>
+        <v>2051</v>
       </c>
       <c r="D34" s="3">
-        <v>0.3219922140419843</v>
+        <v>0.3377943601565521</v>
       </c>
       <c r="E34" s="3">
-        <v>2.181013007639295</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>2.272282415643052</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.936127744510978</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B35" s="2">
-        <v>61.55</v>
+        <v>75.69</v>
       </c>
       <c r="C35" s="3">
-        <v>3185</v>
+        <v>2590</v>
       </c>
       <c r="D35" s="3">
-        <v>0.3226913575222783</v>
+        <v>0.3380101390778742</v>
       </c>
       <c r="E35" s="3">
-        <v>2.178648484142665</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>2.271510940365923</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0.9341317365269461</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B36" s="2">
-        <v>102.59</v>
+        <v>33.83</v>
       </c>
       <c r="C36" s="3">
-        <v>1911</v>
+        <v>5795</v>
       </c>
       <c r="D36" s="3">
-        <v>0.3254989779929619</v>
+        <v>0.3422859857327985</v>
       </c>
       <c r="E36" s="3">
-        <v>2.16915303040582</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>2.256223487991725</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0.9321357285429142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B37" s="2">
-        <v>34.75</v>
+        <v>231.14</v>
       </c>
       <c r="C37" s="3">
-        <v>5642</v>
+        <v>848</v>
       </c>
       <c r="D37" s="3">
-        <v>0.3304873089737303</v>
+        <v>0.3522659804773916</v>
       </c>
       <c r="E37" s="3">
-        <v>2.152282350573362</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>2.220541971168149</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0.9301397205588822</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B38" s="2">
-        <v>93.34</v>
+        <v>60.86</v>
       </c>
       <c r="C38" s="3">
-        <v>2100</v>
+        <v>3221</v>
       </c>
       <c r="D38" s="3">
-        <v>0.3347829165400902</v>
+        <v>0.3533970597332439</v>
       </c>
       <c r="E38" s="3">
-        <v>2.137754481388791</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>2.216498018788479</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.9281437125748504</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B39" s="2">
-        <v>116.85</v>
+        <v>79.14</v>
       </c>
       <c r="C39" s="3">
-        <v>1678</v>
+        <v>2477</v>
       </c>
       <c r="D39" s="3">
-        <v>0.3375394362542766</v>
+        <v>0.3630559001296729</v>
       </c>
       <c r="E39" s="3">
-        <v>2.12843185189023</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>2.175595285446297</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.9261477045908184</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B40" s="2">
-        <v>231.24</v>
+        <v>91.73</v>
       </c>
       <c r="C40" s="3">
-        <v>847</v>
+        <v>2137</v>
       </c>
       <c r="D40" s="3">
-        <v>0.3379570814290284</v>
+        <v>0.3664975149749596</v>
       </c>
       <c r="E40" s="3">
-        <v>2.127019363814765</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>2.169659906538267</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.9241516966067864</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B41" s="2">
-        <v>239.12</v>
+        <v>100.36</v>
       </c>
       <c r="C41" s="3">
-        <v>820</v>
+        <v>1953</v>
       </c>
       <c r="D41" s="3">
-        <v>0.3395003020025645</v>
+        <v>0.3666485425280525</v>
       </c>
       <c r="E41" s="3">
-        <v>2.121800147145429</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>2.169119937097959</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.9221556886227544</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B42" s="2">
-        <v>45.85</v>
+        <v>230.01</v>
       </c>
       <c r="C42" s="3">
-        <v>4276</v>
+        <v>852</v>
       </c>
       <c r="D42" s="3">
-        <v>0.3400629707652693</v>
+        <v>0.3671044613518407</v>
       </c>
       <c r="E42" s="3">
-        <v>2.119897185095815</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>2.16116093323976</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.9201596806387226</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B43" s="2">
-        <v>101.34</v>
+        <v>46.03</v>
       </c>
       <c r="C43" s="3">
-        <v>1934</v>
+        <v>4259</v>
       </c>
       <c r="D43" s="3">
-        <v>0.3424779021632562</v>
+        <v>0.3697786203818231</v>
       </c>
       <c r="E43" s="3">
-        <v>2.111729817174588</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>2.157928956695998</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0.9181636726546907</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B44" s="2">
-        <v>84.77</v>
+        <v>115.42</v>
       </c>
       <c r="C44" s="3">
-        <v>2313</v>
+        <v>1698</v>
       </c>
       <c r="D44" s="3">
-        <v>0.3489260759486069</v>
+        <v>0.3752720048495283</v>
       </c>
       <c r="E44" s="3">
-        <v>2.083411167461392</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>2.138288436303041</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0.9161676646706587</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B45" s="2">
-        <v>65.22</v>
+        <v>41.2</v>
       </c>
       <c r="C45" s="3">
-        <v>3006</v>
+        <v>4759</v>
       </c>
       <c r="D45" s="3">
-        <v>0.3536089691457716</v>
+        <v>0.3786132680438254</v>
       </c>
       <c r="E45" s="3">
-        <v>2.074084226298672</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>2.126342404072523</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0.9141716566866268</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B46" s="2">
-        <v>253.17</v>
+        <v>254.32</v>
       </c>
       <c r="C46" s="3">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="D46" s="3">
-        <v>0.3629005311712583</v>
+        <v>0.3877826926090052</v>
       </c>
       <c r="E46" s="3">
-        <v>2.042659894457069</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>2.093558922191209</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0.9121756487025948</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B47" s="2">
-        <v>62.5</v>
+        <v>114.01</v>
       </c>
       <c r="C47" s="3">
-        <v>3137</v>
+        <v>1719</v>
       </c>
       <c r="D47" s="3">
-        <v>0.3645807589884636</v>
+        <v>0.387855382560884</v>
       </c>
       <c r="E47" s="3">
-        <v>2.036977315322095</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>2.093299033503165</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0.9101796407185628</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B48" s="2">
-        <v>114.43</v>
+        <v>133.19</v>
       </c>
       <c r="C48" s="3">
-        <v>1713</v>
+        <v>1472</v>
       </c>
       <c r="D48" s="3">
-        <v>0.3652869603127575</v>
+        <v>0.3907910315614491</v>
       </c>
       <c r="E48" s="3">
-        <v>2.034588921992672</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>2.082803195390772</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0.9081836327345308</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B49" s="2">
-        <v>69.39</v>
+        <v>66.36</v>
       </c>
       <c r="C49" s="3">
-        <v>2825</v>
+        <v>2954</v>
       </c>
       <c r="D49" s="3">
-        <v>0.3702915697511787</v>
+        <v>0.4015270532790986</v>
       </c>
       <c r="E49" s="3">
-        <v>2.017663187945029</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>2.044418652178049</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0.9061876247504991</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B50" s="2">
-        <v>39.73</v>
+        <v>67.06999999999999</v>
       </c>
       <c r="C50" s="3">
-        <v>4935</v>
+        <v>2923</v>
       </c>
       <c r="D50" s="3">
-        <v>0.3719712908901835</v>
+        <v>0.403513062042743</v>
       </c>
       <c r="E50" s="3">
-        <v>2.011982322410402</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>2.0373180667644</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.9041916167664671</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B51" s="2">
-        <v>132.48</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="C51" s="3">
-        <v>1480</v>
+        <v>2989</v>
       </c>
       <c r="D51" s="3">
-        <v>0.3784074121780183</v>
+        <v>0.4088342922985675</v>
       </c>
       <c r="E51" s="3">
-        <v>1.990215173833343</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>2.018293050043005</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0.9021956087824351</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B52" s="2">
-        <v>29.74</v>
+        <v>28.83</v>
       </c>
       <c r="C52" s="3">
-        <v>6593</v>
+        <v>6801</v>
       </c>
       <c r="D52" s="3">
-        <v>0.3845332481145113</v>
+        <v>0.4082110539894691</v>
       </c>
       <c r="E52" s="3">
-        <v>1.969497419299978</v>
+        <v>2.014603427108114</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0.9001996007984032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>